<commit_message>
Update to Excel Histogram Solution
Start to Excel overlapping histogram solution. Still in progress.
</commit_message>
<xml_diff>
--- a/Seeded Values for Comparison Project.xlsx
+++ b/Seeded Values for Comparison Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\Chart_Comparisons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9775E72-D496-4127-9D07-1218472A85B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564DA6A2-A8E9-4C6F-B070-FDC11F8325F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,21 +17,15 @@
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Data!$A$1:$A$50</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Data!$B$1:$B$50</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Data!$C$1:$C$50</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Data!$A$1:$A$50</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Data!$B$1:$B$50</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Data!$C$1:$C$50</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Data!$C$1:$C$50</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Data!$A$1:$A$50</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Data!$A$1:$A$7</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Data!$A$1:$A$8</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Data!$A$1:$A$9</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Data!$B$1:$B$37</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Data!$B$1:$B$50</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Data!$C$18:$C$21</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Data!$A$1:$A$7</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Data!$B$1:$B$37</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Data!$C$18:$C$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="3" r:id="rId2"/>
+  </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -43,6 +37,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of 37</t>
+  </si>
+  <si>
+    <t>Count of 25</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -79,10 +90,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1344,20 +1360,20 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1396,6 +1412,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00000006-8A65-42DA-85BA-6AFAC922014E}" formatIdx="1">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>Series 1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1409,6 +1426,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{00000007-8A65-42DA-85BA-6AFAC922014E}" formatIdx="0">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>Series 2</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1420,6 +1438,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{00000008-8A65-42DA-85BA-6AFAC922014E}" formatIdx="2">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>Positions</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2690,8 +2709,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3109103" y="6764547"/>
-              <a:ext cx="5916283" cy="3549770"/>
+              <a:off x="3104790" y="6660167"/>
+              <a:ext cx="5907656" cy="3492836"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2722,6 +2741,648 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Vermillion" refreshedDate="44039.851027662036" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="49" xr:uid="{94D777EC-5EAE-4765-84C5-DB1A7F8096E8}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:C50" sheet="Data"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="1" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="50" count="49">
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+        <n v="5"/>
+        <n v="6"/>
+        <n v="7"/>
+        <n v="8"/>
+        <n v="9"/>
+        <n v="10"/>
+        <n v="11"/>
+        <n v="12"/>
+        <n v="13"/>
+        <n v="14"/>
+        <n v="15"/>
+        <n v="16"/>
+        <n v="17"/>
+        <n v="18"/>
+        <n v="19"/>
+        <n v="20"/>
+        <n v="21"/>
+        <n v="22"/>
+        <n v="23"/>
+        <n v="24"/>
+        <n v="25"/>
+        <n v="26"/>
+        <n v="27"/>
+        <n v="28"/>
+        <n v="29"/>
+        <n v="30"/>
+        <n v="31"/>
+        <n v="32"/>
+        <n v="33"/>
+        <n v="34"/>
+        <n v="35"/>
+        <n v="36"/>
+        <n v="37"/>
+        <n v="38"/>
+        <n v="39"/>
+        <n v="40"/>
+        <n v="41"/>
+        <n v="42"/>
+        <n v="43"/>
+        <n v="44"/>
+        <n v="45"/>
+        <n v="46"/>
+        <n v="47"/>
+        <n v="48"/>
+        <n v="49"/>
+        <n v="50"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="37" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="98" count="35">
+        <n v="7"/>
+        <n v="26"/>
+        <n v="27"/>
+        <n v="91"/>
+        <n v="77"/>
+        <n v="58"/>
+        <n v="87"/>
+        <n v="13"/>
+        <n v="62"/>
+        <n v="18"/>
+        <n v="23"/>
+        <n v="61"/>
+        <n v="90"/>
+        <n v="2"/>
+        <n v="54"/>
+        <n v="30"/>
+        <n v="52"/>
+        <n v="39"/>
+        <n v="3"/>
+        <n v="37"/>
+        <n v="32"/>
+        <n v="43"/>
+        <n v="28"/>
+        <n v="6"/>
+        <n v="50"/>
+        <n v="71"/>
+        <n v="45"/>
+        <n v="19"/>
+        <n v="84"/>
+        <n v="46"/>
+        <n v="51"/>
+        <n v="95"/>
+        <n v="16"/>
+        <n v="89"/>
+        <n v="98"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="25" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="100"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="49">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="88"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="65"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="28"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="51"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <n v="29"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="6"/>
+    <n v="83"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="5"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="7"/>
+    <n v="98"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="8"/>
+    <n v="52"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="3"/>
+    <n v="26"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="9"/>
+    <n v="68"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="9"/>
+    <n v="64"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="10"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="11"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="12"/>
+    <n v="39"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="1"/>
+    <n v="53"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="13"/>
+    <n v="96"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <x v="14"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="2"/>
+    <n v="40"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="15"/>
+    <n v="24"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="16"/>
+    <n v="65"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="17"/>
+    <n v="27"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <x v="18"/>
+    <n v="84"/>
+  </r>
+  <r>
+    <x v="24"/>
+    <x v="19"/>
+    <n v="13"/>
+  </r>
+  <r>
+    <x v="25"/>
+    <x v="20"/>
+    <n v="83"/>
+  </r>
+  <r>
+    <x v="26"/>
+    <x v="21"/>
+    <n v="43"/>
+  </r>
+  <r>
+    <x v="27"/>
+    <x v="22"/>
+    <n v="14"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <x v="23"/>
+    <n v="65"/>
+  </r>
+  <r>
+    <x v="29"/>
+    <x v="24"/>
+    <n v="76"/>
+  </r>
+  <r>
+    <x v="30"/>
+    <x v="24"/>
+    <n v="95"/>
+  </r>
+  <r>
+    <x v="31"/>
+    <x v="25"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="32"/>
+    <x v="26"/>
+    <n v="100"/>
+  </r>
+  <r>
+    <x v="33"/>
+    <x v="19"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="34"/>
+    <x v="27"/>
+    <n v="62"/>
+  </r>
+  <r>
+    <x v="35"/>
+    <x v="28"/>
+    <n v="92"/>
+  </r>
+  <r>
+    <x v="36"/>
+    <x v="11"/>
+    <n v="58"/>
+  </r>
+  <r>
+    <x v="37"/>
+    <x v="29"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <x v="38"/>
+    <x v="30"/>
+    <n v="32"/>
+  </r>
+  <r>
+    <x v="39"/>
+    <x v="17"/>
+    <n v="9"/>
+  </r>
+  <r>
+    <x v="40"/>
+    <x v="31"/>
+    <n v="83"/>
+  </r>
+  <r>
+    <x v="41"/>
+    <x v="32"/>
+    <n v="41"/>
+  </r>
+  <r>
+    <x v="42"/>
+    <x v="2"/>
+    <n v="99"/>
+  </r>
+  <r>
+    <x v="43"/>
+    <x v="22"/>
+    <n v="46"/>
+  </r>
+  <r>
+    <x v="44"/>
+    <x v="33"/>
+    <n v="32"/>
+  </r>
+  <r>
+    <x v="45"/>
+    <x v="14"/>
+    <n v="19"/>
+  </r>
+  <r>
+    <x v="46"/>
+    <x v="34"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="47"/>
+    <x v="34"/>
+    <n v="13"/>
+  </r>
+  <r>
+    <x v="48"/>
+    <x v="11"/>
+    <n v="39"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B238523B-94A5-4280-A36D-85B40EFE81DD}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="K6:M56" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="50">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
+      <items count="36">
+        <item x="13"/>
+        <item x="18"/>
+        <item x="23"/>
+        <item x="0"/>
+        <item x="7"/>
+        <item x="32"/>
+        <item x="9"/>
+        <item x="27"/>
+        <item x="10"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="22"/>
+        <item x="15"/>
+        <item x="20"/>
+        <item x="19"/>
+        <item x="17"/>
+        <item x="21"/>
+        <item x="26"/>
+        <item x="29"/>
+        <item x="24"/>
+        <item x="30"/>
+        <item x="16"/>
+        <item x="14"/>
+        <item x="5"/>
+        <item x="11"/>
+        <item x="8"/>
+        <item x="25"/>
+        <item x="4"/>
+        <item x="28"/>
+        <item x="6"/>
+        <item x="33"/>
+        <item x="12"/>
+        <item x="3"/>
+        <item x="31"/>
+        <item x="34"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="50">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Count of 37" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Count of 25" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2925,15 +3586,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="106" workbookViewId="0">
-      <selection sqref="A1:C50"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="46" width="3" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>1</v>
       </c>
@@ -2944,7 +3612,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -2955,7 +3623,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -2966,7 +3634,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -2977,7 +3645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -2988,7 +3656,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -2998,8 +3666,17 @@
       <c r="C6" s="1">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -3009,8 +3686,17 @@
       <c r="C7" s="1">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K7" s="4">
+        <v>2</v>
+      </c>
+      <c r="L7" s="5">
+        <v>1</v>
+      </c>
+      <c r="M7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -3020,8 +3706,17 @@
       <c r="C8" s="1">
         <v>83</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K8" s="4">
+        <v>3</v>
+      </c>
+      <c r="L8" s="5">
+        <v>1</v>
+      </c>
+      <c r="M8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>9</v>
       </c>
@@ -3031,8 +3726,17 @@
       <c r="C9" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K9" s="4">
+        <v>4</v>
+      </c>
+      <c r="L9" s="5">
+        <v>1</v>
+      </c>
+      <c r="M9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>10</v>
       </c>
@@ -3042,8 +3746,17 @@
       <c r="C10" s="1">
         <v>98</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K10" s="4">
+        <v>5</v>
+      </c>
+      <c r="L10" s="5">
+        <v>1</v>
+      </c>
+      <c r="M10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>11</v>
       </c>
@@ -3053,8 +3766,17 @@
       <c r="C11" s="1">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K11" s="4">
+        <v>6</v>
+      </c>
+      <c r="L11" s="5">
+        <v>1</v>
+      </c>
+      <c r="M11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>12</v>
       </c>
@@ -3064,8 +3786,17 @@
       <c r="C12" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K12" s="4">
+        <v>7</v>
+      </c>
+      <c r="L12" s="5">
+        <v>1</v>
+      </c>
+      <c r="M12" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>13</v>
       </c>
@@ -3075,8 +3806,17 @@
       <c r="C13" s="1">
         <v>68</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K13" s="4">
+        <v>8</v>
+      </c>
+      <c r="L13" s="5">
+        <v>1</v>
+      </c>
+      <c r="M13" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>14</v>
       </c>
@@ -3086,8 +3826,17 @@
       <c r="C14" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K14" s="4">
+        <v>9</v>
+      </c>
+      <c r="L14" s="5">
+        <v>1</v>
+      </c>
+      <c r="M14" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>15</v>
       </c>
@@ -3097,8 +3846,17 @@
       <c r="C15" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K15" s="4">
+        <v>10</v>
+      </c>
+      <c r="L15" s="5">
+        <v>1</v>
+      </c>
+      <c r="M15" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>16</v>
       </c>
@@ -3108,8 +3866,17 @@
       <c r="C16" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K16" s="4">
+        <v>11</v>
+      </c>
+      <c r="L16" s="5">
+        <v>1</v>
+      </c>
+      <c r="M16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>17</v>
       </c>
@@ -3119,8 +3886,17 @@
       <c r="C17" s="1">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K17" s="4">
+        <v>12</v>
+      </c>
+      <c r="L17" s="5">
+        <v>1</v>
+      </c>
+      <c r="M17" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>18</v>
       </c>
@@ -3130,8 +3906,17 @@
       <c r="C18" s="1">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K18" s="4">
+        <v>13</v>
+      </c>
+      <c r="L18" s="5">
+        <v>1</v>
+      </c>
+      <c r="M18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>19</v>
       </c>
@@ -3141,8 +3926,17 @@
       <c r="C19" s="1">
         <v>96</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K19" s="4">
+        <v>14</v>
+      </c>
+      <c r="L19" s="5">
+        <v>1</v>
+      </c>
+      <c r="M19" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -3152,8 +3946,17 @@
       <c r="C20" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K20" s="4">
+        <v>15</v>
+      </c>
+      <c r="L20" s="5">
+        <v>1</v>
+      </c>
+      <c r="M20" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -3163,8 +3966,17 @@
       <c r="C21" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K21" s="4">
+        <v>16</v>
+      </c>
+      <c r="L21" s="5">
+        <v>1</v>
+      </c>
+      <c r="M21" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>22</v>
       </c>
@@ -3174,8 +3986,17 @@
       <c r="C22" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K22" s="4">
+        <v>17</v>
+      </c>
+      <c r="L22" s="5">
+        <v>1</v>
+      </c>
+      <c r="M22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>23</v>
       </c>
@@ -3185,8 +4006,17 @@
       <c r="C23" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K23" s="4">
+        <v>18</v>
+      </c>
+      <c r="L23" s="5">
+        <v>1</v>
+      </c>
+      <c r="M23" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>24</v>
       </c>
@@ -3196,8 +4026,17 @@
       <c r="C24" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K24" s="4">
+        <v>19</v>
+      </c>
+      <c r="L24" s="5">
+        <v>1</v>
+      </c>
+      <c r="M24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>25</v>
       </c>
@@ -3207,8 +4046,17 @@
       <c r="C25" s="1">
         <v>84</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K25" s="4">
+        <v>20</v>
+      </c>
+      <c r="L25" s="5">
+        <v>1</v>
+      </c>
+      <c r="M25" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>26</v>
       </c>
@@ -3218,8 +4066,17 @@
       <c r="C26" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K26" s="4">
+        <v>21</v>
+      </c>
+      <c r="L26" s="5">
+        <v>1</v>
+      </c>
+      <c r="M26" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>27</v>
       </c>
@@ -3229,8 +4086,17 @@
       <c r="C27" s="1">
         <v>83</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K27" s="4">
+        <v>22</v>
+      </c>
+      <c r="L27" s="5">
+        <v>1</v>
+      </c>
+      <c r="M27" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>28</v>
       </c>
@@ -3240,8 +4106,17 @@
       <c r="C28" s="1">
         <v>43</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K28" s="4">
+        <v>23</v>
+      </c>
+      <c r="L28" s="5">
+        <v>1</v>
+      </c>
+      <c r="M28" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>29</v>
       </c>
@@ -3251,8 +4126,17 @@
       <c r="C29" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K29" s="4">
+        <v>24</v>
+      </c>
+      <c r="L29" s="5">
+        <v>1</v>
+      </c>
+      <c r="M29" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>30</v>
       </c>
@@ -3262,8 +4146,17 @@
       <c r="C30" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K30" s="4">
+        <v>25</v>
+      </c>
+      <c r="L30" s="5">
+        <v>1</v>
+      </c>
+      <c r="M30" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>31</v>
       </c>
@@ -3273,8 +4166,17 @@
       <c r="C31" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K31" s="4">
+        <v>26</v>
+      </c>
+      <c r="L31" s="5">
+        <v>1</v>
+      </c>
+      <c r="M31" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>32</v>
       </c>
@@ -3284,8 +4186,17 @@
       <c r="C32" s="1">
         <v>95</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K32" s="4">
+        <v>27</v>
+      </c>
+      <c r="L32" s="5">
+        <v>1</v>
+      </c>
+      <c r="M32" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>33</v>
       </c>
@@ -3295,8 +4206,17 @@
       <c r="C33" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K33" s="4">
+        <v>28</v>
+      </c>
+      <c r="L33" s="5">
+        <v>1</v>
+      </c>
+      <c r="M33" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>34</v>
       </c>
@@ -3306,8 +4226,17 @@
       <c r="C34" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K34" s="4">
+        <v>29</v>
+      </c>
+      <c r="L34" s="5">
+        <v>1</v>
+      </c>
+      <c r="M34" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>35</v>
       </c>
@@ -3317,8 +4246,17 @@
       <c r="C35" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K35" s="4">
+        <v>30</v>
+      </c>
+      <c r="L35" s="5">
+        <v>1</v>
+      </c>
+      <c r="M35" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>36</v>
       </c>
@@ -3328,8 +4266,17 @@
       <c r="C36" s="1">
         <v>62</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K36" s="4">
+        <v>31</v>
+      </c>
+      <c r="L36" s="5">
+        <v>1</v>
+      </c>
+      <c r="M36" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>37</v>
       </c>
@@ -3339,8 +4286,17 @@
       <c r="C37" s="1">
         <v>92</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K37" s="4">
+        <v>32</v>
+      </c>
+      <c r="L37" s="5">
+        <v>1</v>
+      </c>
+      <c r="M37" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>38</v>
       </c>
@@ -3350,8 +4306,17 @@
       <c r="C38" s="1">
         <v>58</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K38" s="4">
+        <v>33</v>
+      </c>
+      <c r="L38" s="5">
+        <v>1</v>
+      </c>
+      <c r="M38" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>39</v>
       </c>
@@ -3361,8 +4326,17 @@
       <c r="C39" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K39" s="4">
+        <v>34</v>
+      </c>
+      <c r="L39" s="5">
+        <v>1</v>
+      </c>
+      <c r="M39" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>40</v>
       </c>
@@ -3372,8 +4346,17 @@
       <c r="C40" s="1">
         <v>32</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K40" s="4">
+        <v>35</v>
+      </c>
+      <c r="L40" s="5">
+        <v>1</v>
+      </c>
+      <c r="M40" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>41</v>
       </c>
@@ -3383,8 +4366,17 @@
       <c r="C41" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K41" s="4">
+        <v>36</v>
+      </c>
+      <c r="L41" s="5">
+        <v>1</v>
+      </c>
+      <c r="M41" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>42</v>
       </c>
@@ -3394,8 +4386,17 @@
       <c r="C42" s="1">
         <v>83</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K42" s="4">
+        <v>37</v>
+      </c>
+      <c r="L42" s="5">
+        <v>1</v>
+      </c>
+      <c r="M42" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43</v>
       </c>
@@ -3405,8 +4406,17 @@
       <c r="C43" s="1">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K43" s="4">
+        <v>38</v>
+      </c>
+      <c r="L43" s="5">
+        <v>1</v>
+      </c>
+      <c r="M43" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44</v>
       </c>
@@ -3416,8 +4426,17 @@
       <c r="C44" s="1">
         <v>99</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K44" s="4">
+        <v>39</v>
+      </c>
+      <c r="L44" s="5">
+        <v>1</v>
+      </c>
+      <c r="M44" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>45</v>
       </c>
@@ -3427,8 +4446,17 @@
       <c r="C45" s="1">
         <v>46</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K45" s="4">
+        <v>40</v>
+      </c>
+      <c r="L45" s="5">
+        <v>1</v>
+      </c>
+      <c r="M45" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>46</v>
       </c>
@@ -3438,8 +4466,17 @@
       <c r="C46" s="1">
         <v>32</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K46" s="4">
+        <v>41</v>
+      </c>
+      <c r="L46" s="5">
+        <v>1</v>
+      </c>
+      <c r="M46" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>47</v>
       </c>
@@ -3449,8 +4486,17 @@
       <c r="C47" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K47" s="4">
+        <v>42</v>
+      </c>
+      <c r="L47" s="5">
+        <v>1</v>
+      </c>
+      <c r="M47" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>48</v>
       </c>
@@ -3460,8 +4506,17 @@
       <c r="C48" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K48" s="4">
+        <v>43</v>
+      </c>
+      <c r="L48" s="5">
+        <v>1</v>
+      </c>
+      <c r="M48" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>49</v>
       </c>
@@ -3471,8 +4526,17 @@
       <c r="C49" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K49" s="4">
+        <v>44</v>
+      </c>
+      <c r="L49" s="5">
+        <v>1</v>
+      </c>
+      <c r="M49" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>50</v>
       </c>
@@ -3482,9 +4546,84 @@
       <c r="C50" s="1">
         <v>39</v>
       </c>
+      <c r="K50" s="4">
+        <v>45</v>
+      </c>
+      <c r="L50" s="5">
+        <v>1</v>
+      </c>
+      <c r="M50" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K51" s="4">
+        <v>46</v>
+      </c>
+      <c r="L51" s="5">
+        <v>1</v>
+      </c>
+      <c r="M51" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K52" s="4">
+        <v>47</v>
+      </c>
+      <c r="L52" s="5">
+        <v>1</v>
+      </c>
+      <c r="M52" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K53" s="4">
+        <v>48</v>
+      </c>
+      <c r="L53" s="5">
+        <v>1</v>
+      </c>
+      <c r="M53" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K54" s="4">
+        <v>49</v>
+      </c>
+      <c r="L54" s="5">
+        <v>1</v>
+      </c>
+      <c r="M54" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K55" s="4">
+        <v>50</v>
+      </c>
+      <c r="L55" s="5">
+        <v>1</v>
+      </c>
+      <c r="M55" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K56" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L56" s="5">
+        <v>49</v>
+      </c>
+      <c r="M56" s="5">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to .odt and .xlsx
Attempted to finish histogram in Excel, but it is proving challenging. Will return later for a different attempt.
</commit_message>
<xml_diff>
--- a/Seeded Values for Comparison Project.xlsx
+++ b/Seeded Values for Comparison Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\Chart_Comparisons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564DA6A2-A8E9-4C6F-B070-FDC11F8325F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CDD3A1-E45C-4428-A01D-F0301FFC2A1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,16 +16,15 @@
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Data!$A$1:$A$50</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Data!$A$1:$A$7</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Data!$B$1:$B$37</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Data!$C$18:$C$21</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Data!$A$2:$A$51</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Data!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Data!$B$2:$B$38</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Data!$C$19:$C$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId2"/>
+    <pivotCache cacheId="5" r:id="rId2"/>
   </pivotCaches>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Row Labels</t>
   </si>
@@ -48,10 +47,34 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>Count of 37</t>
+    <t>Labels</t>
   </si>
   <si>
-    <t>Count of 25</t>
+    <t>Series 1</t>
+  </si>
+  <si>
+    <t>Series 2</t>
+  </si>
+  <si>
+    <t>Count of Series 1</t>
+  </si>
+  <si>
+    <t>Count of Series 2</t>
+  </si>
+  <si>
+    <t>1-10</t>
+  </si>
+  <si>
+    <t>11-20</t>
+  </si>
+  <si>
+    <t>21-30</t>
+  </si>
+  <si>
+    <t>31-40</t>
+  </si>
+  <si>
+    <t>41-50</t>
   </si>
 </sst>
 </file>
@@ -270,7 +293,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$A$1:$A$50</c:f>
+              <c:f>Data!$A$2:$A$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -429,7 +452,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$B$1:$B$50</c:f>
+              <c:f>Data!$B$2:$B$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -704,7 +727,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$A$1:$A$50</c:f>
+              <c:f>Data!$A$2:$A$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -863,7 +886,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$C$1:$C$50</c:f>
+              <c:f>Data!$C$2:$C$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -1202,6 +1225,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.7734168648640622E-3"/>
+              <c:y val="1.0690486342706572E-3"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2630,13 +2661,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>597491</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>216491</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>11430</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2666,13 +2697,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>132990</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>122207</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>97046</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>48883</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2709,8 +2740,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3104790" y="6660167"/>
-              <a:ext cx="5907656" cy="3492836"/>
+              <a:off x="3104790" y="5654327"/>
+              <a:ext cx="5907656" cy="2974676"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2744,13 +2775,14 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Vermillion" refreshedDate="44039.851027662036" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="49" xr:uid="{94D777EC-5EAE-4765-84C5-DB1A7F8096E8}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Vermillion" refreshedDate="44041.841485648147" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="50" xr:uid="{7194D51C-B0D7-4FB2-A473-4F942CE2C998}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:C50" sheet="Data"/>
+    <worksheetSource ref="A1:C51" sheet="Data"/>
   </cacheSource>
   <cacheFields count="3">
-    <cacheField name="1" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="50" count="49">
+    <cacheField name="Labels" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="50" count="50">
+        <n v="1"/>
         <n v="2"/>
         <n v="3"/>
         <n v="4"/>
@@ -2801,47 +2833,28 @@
         <n v="49"/>
         <n v="50"/>
       </sharedItems>
+      <fieldGroup base="0">
+        <rangePr autoEnd="0" startNum="1" endNum="100" groupInterval="10"/>
+        <groupItems count="12">
+          <s v="&lt;1"/>
+          <s v="1-10"/>
+          <s v="11-20"/>
+          <s v="21-30"/>
+          <s v="31-40"/>
+          <s v="41-50"/>
+          <s v="51-60"/>
+          <s v="61-70"/>
+          <s v="71-80"/>
+          <s v="81-90"/>
+          <s v="91-100"/>
+          <s v="&gt;101"/>
+        </groupItems>
+      </fieldGroup>
     </cacheField>
-    <cacheField name="37" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="98" count="35">
-        <n v="7"/>
-        <n v="26"/>
-        <n v="27"/>
-        <n v="91"/>
-        <n v="77"/>
-        <n v="58"/>
-        <n v="87"/>
-        <n v="13"/>
-        <n v="62"/>
-        <n v="18"/>
-        <n v="23"/>
-        <n v="61"/>
-        <n v="90"/>
-        <n v="2"/>
-        <n v="54"/>
-        <n v="30"/>
-        <n v="52"/>
-        <n v="39"/>
-        <n v="3"/>
-        <n v="37"/>
-        <n v="32"/>
-        <n v="43"/>
-        <n v="28"/>
-        <n v="6"/>
-        <n v="50"/>
-        <n v="71"/>
-        <n v="45"/>
-        <n v="19"/>
-        <n v="84"/>
-        <n v="46"/>
-        <n v="51"/>
-        <n v="95"/>
-        <n v="16"/>
-        <n v="89"/>
-        <n v="98"/>
-      </sharedItems>
+    <cacheField name="Series 1" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="98"/>
     </cacheField>
-    <cacheField name="25" numFmtId="0">
+    <cacheField name="Series 2" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="100"/>
     </cacheField>
   </cacheFields>
@@ -2854,261 +2867,266 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="49">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="50">
   <r>
     <x v="0"/>
-    <x v="0"/>
+    <n v="37"/>
+    <n v="25"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="7"/>
     <n v="88"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="2"/>
+    <n v="26"/>
     <n v="65"/>
   </r>
   <r>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="3"/>
+    <n v="27"/>
     <n v="5"/>
   </r>
   <r>
-    <x v="3"/>
-    <x v="3"/>
+    <x v="4"/>
+    <n v="91"/>
     <n v="28"/>
   </r>
   <r>
-    <x v="4"/>
-    <x v="4"/>
+    <x v="5"/>
+    <n v="77"/>
     <n v="51"/>
   </r>
   <r>
-    <x v="5"/>
-    <x v="5"/>
+    <x v="6"/>
+    <n v="58"/>
     <n v="29"/>
   </r>
   <r>
-    <x v="6"/>
-    <x v="6"/>
+    <x v="7"/>
+    <n v="87"/>
     <n v="83"/>
   </r>
   <r>
-    <x v="7"/>
-    <x v="5"/>
+    <x v="8"/>
+    <n v="58"/>
     <n v="10"/>
   </r>
   <r>
-    <x v="8"/>
-    <x v="7"/>
+    <x v="9"/>
+    <n v="13"/>
     <n v="98"/>
   </r>
   <r>
-    <x v="9"/>
-    <x v="8"/>
+    <x v="10"/>
+    <n v="62"/>
     <n v="52"/>
   </r>
   <r>
-    <x v="10"/>
-    <x v="3"/>
+    <x v="11"/>
+    <n v="91"/>
     <n v="26"/>
   </r>
   <r>
-    <x v="11"/>
-    <x v="9"/>
+    <x v="12"/>
+    <n v="18"/>
     <n v="68"/>
   </r>
   <r>
-    <x v="12"/>
-    <x v="9"/>
+    <x v="13"/>
+    <n v="18"/>
     <n v="64"/>
   </r>
   <r>
-    <x v="13"/>
-    <x v="10"/>
+    <x v="14"/>
+    <n v="23"/>
     <n v="3"/>
   </r>
   <r>
-    <x v="14"/>
-    <x v="11"/>
+    <x v="15"/>
+    <n v="61"/>
     <n v="6"/>
   </r>
   <r>
-    <x v="15"/>
-    <x v="12"/>
+    <x v="16"/>
+    <n v="90"/>
     <n v="39"/>
   </r>
   <r>
-    <x v="16"/>
-    <x v="1"/>
+    <x v="17"/>
+    <n v="26"/>
     <n v="53"/>
   </r>
   <r>
-    <x v="17"/>
-    <x v="13"/>
+    <x v="18"/>
+    <n v="2"/>
     <n v="96"/>
   </r>
   <r>
-    <x v="18"/>
-    <x v="14"/>
+    <x v="19"/>
+    <n v="54"/>
     <n v="15"/>
   </r>
   <r>
-    <x v="19"/>
-    <x v="2"/>
+    <x v="20"/>
+    <n v="27"/>
     <n v="40"/>
   </r>
   <r>
-    <x v="20"/>
-    <x v="15"/>
+    <x v="21"/>
+    <n v="30"/>
     <n v="24"/>
   </r>
   <r>
-    <x v="21"/>
-    <x v="16"/>
+    <x v="22"/>
+    <n v="52"/>
     <n v="65"/>
   </r>
   <r>
-    <x v="22"/>
-    <x v="17"/>
+    <x v="23"/>
+    <n v="39"/>
     <n v="27"/>
   </r>
   <r>
-    <x v="23"/>
-    <x v="18"/>
+    <x v="24"/>
+    <n v="3"/>
     <n v="84"/>
   </r>
   <r>
-    <x v="24"/>
-    <x v="19"/>
+    <x v="25"/>
+    <n v="37"/>
     <n v="13"/>
   </r>
   <r>
-    <x v="25"/>
-    <x v="20"/>
+    <x v="26"/>
+    <n v="32"/>
     <n v="83"/>
   </r>
   <r>
-    <x v="26"/>
-    <x v="21"/>
+    <x v="27"/>
     <n v="43"/>
-  </r>
-  <r>
-    <x v="27"/>
-    <x v="22"/>
+    <n v="43"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <n v="28"/>
     <n v="14"/>
   </r>
   <r>
-    <x v="28"/>
-    <x v="23"/>
+    <x v="29"/>
+    <n v="6"/>
     <n v="65"/>
   </r>
   <r>
-    <x v="29"/>
-    <x v="24"/>
+    <x v="30"/>
+    <n v="50"/>
     <n v="76"/>
   </r>
   <r>
-    <x v="30"/>
-    <x v="24"/>
+    <x v="31"/>
+    <n v="50"/>
     <n v="95"/>
   </r>
   <r>
-    <x v="31"/>
-    <x v="25"/>
+    <x v="32"/>
+    <n v="71"/>
     <n v="15"/>
   </r>
   <r>
-    <x v="32"/>
-    <x v="26"/>
+    <x v="33"/>
+    <n v="45"/>
     <n v="100"/>
   </r>
   <r>
-    <x v="33"/>
-    <x v="19"/>
+    <x v="34"/>
+    <n v="37"/>
     <n v="5"/>
   </r>
   <r>
-    <x v="34"/>
-    <x v="27"/>
+    <x v="35"/>
+    <n v="19"/>
     <n v="62"/>
   </r>
   <r>
-    <x v="35"/>
-    <x v="28"/>
+    <x v="36"/>
+    <n v="84"/>
     <n v="92"/>
   </r>
   <r>
-    <x v="36"/>
-    <x v="11"/>
+    <x v="37"/>
+    <n v="61"/>
     <n v="58"/>
   </r>
   <r>
-    <x v="37"/>
-    <x v="29"/>
+    <x v="38"/>
+    <n v="46"/>
     <n v="10"/>
   </r>
   <r>
-    <x v="38"/>
-    <x v="30"/>
+    <x v="39"/>
+    <n v="51"/>
     <n v="32"/>
   </r>
   <r>
-    <x v="39"/>
-    <x v="17"/>
+    <x v="40"/>
+    <n v="39"/>
     <n v="9"/>
   </r>
   <r>
-    <x v="40"/>
-    <x v="31"/>
+    <x v="41"/>
+    <n v="95"/>
     <n v="83"/>
   </r>
   <r>
-    <x v="41"/>
-    <x v="32"/>
+    <x v="42"/>
+    <n v="16"/>
     <n v="41"/>
   </r>
   <r>
-    <x v="42"/>
-    <x v="2"/>
+    <x v="43"/>
+    <n v="27"/>
     <n v="99"/>
   </r>
   <r>
-    <x v="43"/>
-    <x v="22"/>
+    <x v="44"/>
+    <n v="28"/>
     <n v="46"/>
   </r>
   <r>
-    <x v="44"/>
-    <x v="33"/>
+    <x v="45"/>
+    <n v="89"/>
     <n v="32"/>
   </r>
   <r>
-    <x v="45"/>
-    <x v="14"/>
+    <x v="46"/>
+    <n v="54"/>
     <n v="19"/>
   </r>
   <r>
-    <x v="46"/>
-    <x v="34"/>
+    <x v="47"/>
+    <n v="98"/>
     <n v="1"/>
   </r>
   <r>
-    <x v="47"/>
-    <x v="34"/>
+    <x v="48"/>
+    <n v="98"/>
     <n v="13"/>
   </r>
   <r>
-    <x v="48"/>
-    <x v="11"/>
+    <x v="49"/>
+    <n v="61"/>
     <n v="39"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B238523B-94A5-4280-A36D-85B40EFE81DD}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="K6:M56" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{38C5BB80-E974-42CE-9DD0-85C2AC69A4FC}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="K6:M12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
-      <items count="50">
+      <items count="13">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -3121,95 +3139,16 @@
         <item x="9"/>
         <item x="10"/>
         <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="35"/>
-        <item x="36"/>
-        <item x="37"/>
-        <item x="38"/>
-        <item x="39"/>
-        <item x="40"/>
-        <item x="41"/>
-        <item x="42"/>
-        <item x="43"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item x="46"/>
-        <item x="47"/>
-        <item x="48"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" showAll="0">
-      <items count="36">
-        <item x="13"/>
-        <item x="18"/>
-        <item x="23"/>
-        <item x="0"/>
-        <item x="7"/>
-        <item x="32"/>
-        <item x="9"/>
-        <item x="27"/>
-        <item x="10"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="22"/>
-        <item x="15"/>
-        <item x="20"/>
-        <item x="19"/>
-        <item x="17"/>
-        <item x="21"/>
-        <item x="26"/>
-        <item x="29"/>
-        <item x="24"/>
-        <item x="30"/>
-        <item x="16"/>
-        <item x="14"/>
-        <item x="5"/>
-        <item x="11"/>
-        <item x="8"/>
-        <item x="25"/>
-        <item x="4"/>
-        <item x="28"/>
-        <item x="6"/>
-        <item x="33"/>
-        <item x="12"/>
-        <item x="3"/>
-        <item x="31"/>
-        <item x="34"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="50">
-    <i>
-      <x/>
-    </i>
+  <rowItems count="6">
     <i>
       <x v="1"/>
     </i>
@@ -3224,135 +3163,6 @@
     </i>
     <i>
       <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="33"/>
-    </i>
-    <i>
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="35"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="39"/>
-    </i>
-    <i>
-      <x v="40"/>
-    </i>
-    <i>
-      <x v="41"/>
-    </i>
-    <i>
-      <x v="42"/>
-    </i>
-    <i>
-      <x v="43"/>
-    </i>
-    <i>
-      <x v="44"/>
-    </i>
-    <i>
-      <x v="45"/>
-    </i>
-    <i>
-      <x v="46"/>
-    </i>
-    <i>
-      <x v="47"/>
-    </i>
-    <i>
-      <x v="48"/>
     </i>
     <i t="grand">
       <x/>
@@ -3370,8 +3180,8 @@
     </i>
   </colItems>
   <dataFields count="2">
-    <dataField name="Count of 37" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Count of 25" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Count of Series 1" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Count of Series 2" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -3586,1040 +3396,643 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="11" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="2" bestFit="1" customWidth="1"/>
     <col min="16" max="46" width="3" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B2" s="1">
         <v>37</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C2" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="3" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1">
         <v>7</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C3" s="1">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="4" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>26</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C4" s="1">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="5" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>27</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="6" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>91</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="1">
         <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>77</v>
-      </c>
-      <c r="C6" s="1">
-        <v>51</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>77</v>
+      </c>
+      <c r="C7" s="1">
+        <v>51</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1">
+      <c r="L7" s="5">
+        <v>10</v>
+      </c>
+      <c r="M7" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
         <v>58</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="1">
         <v>29</v>
       </c>
-      <c r="K7" s="4">
-        <v>2</v>
-      </c>
-      <c r="L7" s="5">
+      <c r="K8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" s="5">
+        <v>10</v>
+      </c>
+      <c r="M8" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>87</v>
+      </c>
+      <c r="C9" s="1">
+        <v>83</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="5">
+        <v>10</v>
+      </c>
+      <c r="M9" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>58</v>
+      </c>
+      <c r="C10" s="1">
+        <v>10</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="5">
+        <v>10</v>
+      </c>
+      <c r="M10" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1">
+        <v>98</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="5">
+        <v>10</v>
+      </c>
+      <c r="M11" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>62</v>
+      </c>
+      <c r="C12" s="1">
+        <v>52</v>
+      </c>
+      <c r="K12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="M7" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1">
-        <v>87</v>
-      </c>
-      <c r="C8" s="1">
-        <v>83</v>
-      </c>
-      <c r="K8" s="4">
-        <v>3</v>
-      </c>
-      <c r="L8" s="5">
-        <v>1</v>
-      </c>
-      <c r="M8" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1">
-        <v>58</v>
-      </c>
-      <c r="C9" s="1">
-        <v>10</v>
-      </c>
-      <c r="K9" s="4">
-        <v>4</v>
-      </c>
-      <c r="L9" s="5">
-        <v>1</v>
-      </c>
-      <c r="M9" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1">
+      <c r="L12" s="5">
+        <v>50</v>
+      </c>
+      <c r="M12" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>91</v>
+      </c>
+      <c r="C13" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>13</v>
-      </c>
-      <c r="C10" s="1">
-        <v>98</v>
-      </c>
-      <c r="K10" s="4">
-        <v>5</v>
-      </c>
-      <c r="L10" s="5">
-        <v>1</v>
-      </c>
-      <c r="M10" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1">
-        <v>62</v>
-      </c>
-      <c r="C11" s="1">
-        <v>52</v>
-      </c>
-      <c r="K11" s="4">
-        <v>6</v>
-      </c>
-      <c r="L11" s="5">
-        <v>1</v>
-      </c>
-      <c r="M11" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1">
-        <v>91</v>
-      </c>
-      <c r="C12" s="1">
-        <v>26</v>
-      </c>
-      <c r="K12" s="4">
-        <v>7</v>
-      </c>
-      <c r="L12" s="5">
-        <v>1</v>
-      </c>
-      <c r="M12" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1">
-        <v>18</v>
-      </c>
-      <c r="C13" s="1">
-        <v>68</v>
-      </c>
-      <c r="K13" s="4">
-        <v>8</v>
-      </c>
-      <c r="L13" s="5">
-        <v>1</v>
-      </c>
-      <c r="M13" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>18</v>
       </c>
       <c r="C14" s="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1">
         <v>64</v>
       </c>
-      <c r="K14" s="4">
-        <v>9</v>
-      </c>
-      <c r="L14" s="5">
-        <v>1</v>
-      </c>
-      <c r="M14" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    </row>
+    <row r="16" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B16" s="1">
         <v>23</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C16" s="1">
         <v>3</v>
       </c>
-      <c r="K15" s="4">
-        <v>10</v>
-      </c>
-      <c r="L15" s="5">
-        <v>1</v>
-      </c>
-      <c r="M15" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+    </row>
+    <row r="17" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B17" s="1">
         <v>61</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C17" s="1">
         <v>6</v>
       </c>
-      <c r="K16" s="4">
-        <v>11</v>
-      </c>
-      <c r="L16" s="5">
-        <v>1</v>
-      </c>
-      <c r="M16" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+    </row>
+    <row r="18" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B18" s="1">
         <v>90</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C18" s="1">
         <v>39</v>
       </c>
-      <c r="K17" s="4">
-        <v>12</v>
-      </c>
-      <c r="L17" s="5">
-        <v>1</v>
-      </c>
-      <c r="M17" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+    </row>
+    <row r="19" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B19" s="1">
         <v>26</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C19" s="1">
         <v>53</v>
       </c>
-      <c r="K18" s="4">
+    </row>
+    <row r="20" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>54</v>
+      </c>
+      <c r="C21" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>27</v>
+      </c>
+      <c r="C22" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>30</v>
+      </c>
+      <c r="C23" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>52</v>
+      </c>
+      <c r="C24" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>39</v>
+      </c>
+      <c r="C25" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>37</v>
+      </c>
+      <c r="C27" s="1">
         <v>13</v>
       </c>
-      <c r="L18" s="5">
-        <v>1</v>
-      </c>
-      <c r="M18" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>19</v>
-      </c>
-      <c r="B19" s="1">
-        <v>2</v>
-      </c>
-      <c r="C19" s="1">
-        <v>96</v>
-      </c>
-      <c r="K19" s="4">
+    </row>
+    <row r="28" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>32</v>
+      </c>
+      <c r="C28" s="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1">
+        <v>43</v>
+      </c>
+      <c r="C29" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1">
+        <v>28</v>
+      </c>
+      <c r="C30" s="1">
         <v>14</v>
       </c>
-      <c r="L19" s="5">
-        <v>1</v>
-      </c>
-      <c r="M19" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>20</v>
-      </c>
-      <c r="B20" s="1">
-        <v>54</v>
-      </c>
-      <c r="C20" s="1">
-        <v>15</v>
-      </c>
-      <c r="K20" s="4">
-        <v>15</v>
-      </c>
-      <c r="L20" s="5">
-        <v>1</v>
-      </c>
-      <c r="M20" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>21</v>
-      </c>
-      <c r="B21" s="1">
-        <v>27</v>
-      </c>
-      <c r="C21" s="1">
-        <v>40</v>
-      </c>
-      <c r="K21" s="4">
-        <v>16</v>
-      </c>
-      <c r="L21" s="5">
-        <v>1</v>
-      </c>
-      <c r="M21" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>22</v>
-      </c>
-      <c r="B22" s="1">
+    </row>
+    <row r="31" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="C22" s="1">
-        <v>24</v>
-      </c>
-      <c r="K22" s="4">
-        <v>17</v>
-      </c>
-      <c r="L22" s="5">
-        <v>1</v>
-      </c>
-      <c r="M22" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>23</v>
-      </c>
-      <c r="B23" s="1">
-        <v>52</v>
-      </c>
-      <c r="C23" s="1">
+      <c r="B31" s="1">
+        <v>6</v>
+      </c>
+      <c r="C31" s="1">
         <v>65</v>
       </c>
-      <c r="K23" s="4">
-        <v>18</v>
-      </c>
-      <c r="L23" s="5">
-        <v>1</v>
-      </c>
-      <c r="M23" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1">
-        <v>39</v>
-      </c>
-      <c r="C24" s="1">
-        <v>27</v>
-      </c>
-      <c r="K24" s="4">
-        <v>19</v>
-      </c>
-      <c r="L24" s="5">
-        <v>1</v>
-      </c>
-      <c r="M24" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>25</v>
-      </c>
-      <c r="B25" s="1">
-        <v>3</v>
-      </c>
-      <c r="C25" s="1">
-        <v>84</v>
-      </c>
-      <c r="K25" s="4">
-        <v>20</v>
-      </c>
-      <c r="L25" s="5">
-        <v>1</v>
-      </c>
-      <c r="M25" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>26</v>
-      </c>
-      <c r="B26" s="1">
-        <v>37</v>
-      </c>
-      <c r="C26" s="1">
-        <v>13</v>
-      </c>
-      <c r="K26" s="4">
-        <v>21</v>
-      </c>
-      <c r="L26" s="5">
-        <v>1</v>
-      </c>
-      <c r="M26" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>27</v>
-      </c>
-      <c r="B27" s="1">
-        <v>32</v>
-      </c>
-      <c r="C27" s="1">
-        <v>83</v>
-      </c>
-      <c r="K27" s="4">
-        <v>22</v>
-      </c>
-      <c r="L27" s="5">
-        <v>1</v>
-      </c>
-      <c r="M27" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>28</v>
-      </c>
-      <c r="B28" s="1">
-        <v>43</v>
-      </c>
-      <c r="C28" s="1">
-        <v>43</v>
-      </c>
-      <c r="K28" s="4">
-        <v>23</v>
-      </c>
-      <c r="L28" s="5">
-        <v>1</v>
-      </c>
-      <c r="M28" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>29</v>
-      </c>
-      <c r="B29" s="1">
-        <v>28</v>
-      </c>
-      <c r="C29" s="1">
-        <v>14</v>
-      </c>
-      <c r="K29" s="4">
-        <v>24</v>
-      </c>
-      <c r="L29" s="5">
-        <v>1</v>
-      </c>
-      <c r="M29" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>30</v>
-      </c>
-      <c r="B30" s="1">
-        <v>6</v>
-      </c>
-      <c r="C30" s="1">
-        <v>65</v>
-      </c>
-      <c r="K30" s="4">
-        <v>25</v>
-      </c>
-      <c r="L30" s="5">
-        <v>1</v>
-      </c>
-      <c r="M30" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+    </row>
+    <row r="32" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>31</v>
-      </c>
-      <c r="B31" s="1">
-        <v>50</v>
-      </c>
-      <c r="C31" s="1">
-        <v>76</v>
-      </c>
-      <c r="K31" s="4">
-        <v>26</v>
-      </c>
-      <c r="L31" s="5">
-        <v>1</v>
-      </c>
-      <c r="M31" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>32</v>
       </c>
       <c r="B32" s="1">
         <v>50</v>
       </c>
       <c r="C32" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1">
+        <v>50</v>
+      </c>
+      <c r="C33" s="1">
         <v>95</v>
       </c>
-      <c r="K32" s="4">
+    </row>
+    <row r="34" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1">
+        <v>71</v>
+      </c>
+      <c r="C34" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1">
+        <v>45</v>
+      </c>
+      <c r="C35" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1">
+        <v>37</v>
+      </c>
+      <c r="C36" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1">
+        <v>19</v>
+      </c>
+      <c r="C37" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1">
+        <v>84</v>
+      </c>
+      <c r="C38" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1">
+        <v>61</v>
+      </c>
+      <c r="C39" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1">
+        <v>46</v>
+      </c>
+      <c r="C40" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1">
+        <v>51</v>
+      </c>
+      <c r="C41" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1">
+        <v>39</v>
+      </c>
+      <c r="C42" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1">
+        <v>95</v>
+      </c>
+      <c r="C43" s="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1">
+        <v>16</v>
+      </c>
+      <c r="C44" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1">
         <v>27</v>
       </c>
-      <c r="L32" s="5">
-        <v>1</v>
-      </c>
-      <c r="M32" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>33</v>
-      </c>
-      <c r="B33" s="1">
-        <v>71</v>
-      </c>
-      <c r="C33" s="1">
-        <v>15</v>
-      </c>
-      <c r="K33" s="4">
+      <c r="C45" s="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1">
         <v>28</v>
       </c>
-      <c r="L33" s="5">
-        <v>1</v>
-      </c>
-      <c r="M33" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>34</v>
-      </c>
-      <c r="B34" s="1">
-        <v>45</v>
-      </c>
-      <c r="C34" s="1">
-        <v>100</v>
-      </c>
-      <c r="K34" s="4">
-        <v>29</v>
-      </c>
-      <c r="L34" s="5">
-        <v>1</v>
-      </c>
-      <c r="M34" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>35</v>
-      </c>
-      <c r="B35" s="1">
-        <v>37</v>
-      </c>
-      <c r="C35" s="1">
-        <v>5</v>
-      </c>
-      <c r="K35" s="4">
-        <v>30</v>
-      </c>
-      <c r="L35" s="5">
-        <v>1</v>
-      </c>
-      <c r="M35" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>36</v>
-      </c>
-      <c r="B36" s="1">
+      <c r="C46" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1">
+        <v>89</v>
+      </c>
+      <c r="C47" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1">
+        <v>54</v>
+      </c>
+      <c r="C48" s="1">
         <v>19</v>
       </c>
-      <c r="C36" s="1">
-        <v>62</v>
-      </c>
-      <c r="K36" s="4">
-        <v>31</v>
-      </c>
-      <c r="L36" s="5">
-        <v>1</v>
-      </c>
-      <c r="M36" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>37</v>
-      </c>
-      <c r="B37" s="1">
-        <v>84</v>
-      </c>
-      <c r="C37" s="1">
-        <v>92</v>
-      </c>
-      <c r="K37" s="4">
-        <v>32</v>
-      </c>
-      <c r="L37" s="5">
-        <v>1</v>
-      </c>
-      <c r="M37" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>38</v>
-      </c>
-      <c r="B38" s="1">
-        <v>61</v>
-      </c>
-      <c r="C38" s="1">
-        <v>58</v>
-      </c>
-      <c r="K38" s="4">
-        <v>33</v>
-      </c>
-      <c r="L38" s="5">
-        <v>1</v>
-      </c>
-      <c r="M38" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>39</v>
-      </c>
-      <c r="B39" s="1">
-        <v>46</v>
-      </c>
-      <c r="C39" s="1">
-        <v>10</v>
-      </c>
-      <c r="K39" s="4">
-        <v>34</v>
-      </c>
-      <c r="L39" s="5">
-        <v>1</v>
-      </c>
-      <c r="M39" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>40</v>
-      </c>
-      <c r="B40" s="1">
-        <v>51</v>
-      </c>
-      <c r="C40" s="1">
-        <v>32</v>
-      </c>
-      <c r="K40" s="4">
-        <v>35</v>
-      </c>
-      <c r="L40" s="5">
-        <v>1</v>
-      </c>
-      <c r="M40" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>41</v>
-      </c>
-      <c r="B41" s="1">
-        <v>39</v>
-      </c>
-      <c r="C41" s="1">
-        <v>9</v>
-      </c>
-      <c r="K41" s="4">
-        <v>36</v>
-      </c>
-      <c r="L41" s="5">
-        <v>1</v>
-      </c>
-      <c r="M41" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>42</v>
-      </c>
-      <c r="B42" s="1">
-        <v>95</v>
-      </c>
-      <c r="C42" s="1">
-        <v>83</v>
-      </c>
-      <c r="K42" s="4">
-        <v>37</v>
-      </c>
-      <c r="L42" s="5">
-        <v>1</v>
-      </c>
-      <c r="M42" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>43</v>
-      </c>
-      <c r="B43" s="1">
-        <v>16</v>
-      </c>
-      <c r="C43" s="1">
-        <v>41</v>
-      </c>
-      <c r="K43" s="4">
-        <v>38</v>
-      </c>
-      <c r="L43" s="5">
-        <v>1</v>
-      </c>
-      <c r="M43" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>44</v>
-      </c>
-      <c r="B44" s="1">
-        <v>27</v>
-      </c>
-      <c r="C44" s="1">
-        <v>99</v>
-      </c>
-      <c r="K44" s="4">
-        <v>39</v>
-      </c>
-      <c r="L44" s="5">
-        <v>1</v>
-      </c>
-      <c r="M44" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>45</v>
-      </c>
-      <c r="B45" s="1">
-        <v>28</v>
-      </c>
-      <c r="C45" s="1">
-        <v>46</v>
-      </c>
-      <c r="K45" s="4">
-        <v>40</v>
-      </c>
-      <c r="L45" s="5">
-        <v>1</v>
-      </c>
-      <c r="M45" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>46</v>
-      </c>
-      <c r="B46" s="1">
-        <v>89</v>
-      </c>
-      <c r="C46" s="1">
-        <v>32</v>
-      </c>
-      <c r="K46" s="4">
-        <v>41</v>
-      </c>
-      <c r="L46" s="5">
-        <v>1</v>
-      </c>
-      <c r="M46" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>47</v>
-      </c>
-      <c r="B47" s="1">
-        <v>54</v>
-      </c>
-      <c r="C47" s="1">
-        <v>19</v>
-      </c>
-      <c r="K47" s="4">
-        <v>42</v>
-      </c>
-      <c r="L47" s="5">
-        <v>1</v>
-      </c>
-      <c r="M47" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+    </row>
+    <row r="49" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
         <v>48</v>
-      </c>
-      <c r="B48" s="1">
-        <v>98</v>
-      </c>
-      <c r="C48" s="1">
-        <v>1</v>
-      </c>
-      <c r="K48" s="4">
-        <v>43</v>
-      </c>
-      <c r="L48" s="5">
-        <v>1</v>
-      </c>
-      <c r="M48" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>49</v>
       </c>
       <c r="B49" s="1">
         <v>98</v>
       </c>
       <c r="C49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1">
+        <v>98</v>
+      </c>
+      <c r="C50" s="1">
         <v>13</v>
       </c>
-      <c r="K49" s="4">
-        <v>44</v>
-      </c>
-      <c r="L49" s="5">
-        <v>1</v>
-      </c>
-      <c r="M49" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+    </row>
+    <row r="51" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B51" s="1">
         <v>61</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C51" s="1">
         <v>39</v>
-      </c>
-      <c r="K50" s="4">
-        <v>45</v>
-      </c>
-      <c r="L50" s="5">
-        <v>1</v>
-      </c>
-      <c r="M50" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K51" s="4">
-        <v>46</v>
-      </c>
-      <c r="L51" s="5">
-        <v>1</v>
-      </c>
-      <c r="M51" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K52" s="4">
-        <v>47</v>
-      </c>
-      <c r="L52" s="5">
-        <v>1</v>
-      </c>
-      <c r="M52" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K53" s="4">
-        <v>48</v>
-      </c>
-      <c r="L53" s="5">
-        <v>1</v>
-      </c>
-      <c r="M53" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K54" s="4">
-        <v>49</v>
-      </c>
-      <c r="L54" s="5">
-        <v>1</v>
-      </c>
-      <c r="M54" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K55" s="4">
-        <v>50</v>
-      </c>
-      <c r="L55" s="5">
-        <v>1</v>
-      </c>
-      <c r="M55" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K56" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L56" s="5">
-        <v>49</v>
-      </c>
-      <c r="M56" s="5">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Excel Double Histogram
I tried three separate solution attempts before arriving on the one presented. The default spacing was atrocious, so that was changed. Everything else was as close to default as possible.
</commit_message>
<xml_diff>
--- a/Seeded Values for Comparison Project.xlsx
+++ b/Seeded Values for Comparison Project.xlsx
@@ -1,29 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\Chart_Comparisons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CDD3A1-E45C-4428-A01D-F0301FFC2A1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5832953A-B6F8-4CA9-B2B6-743BA277FC93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="2" r:id="rId1"/>
+    <sheet name="Data (2)" sheetId="3" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Data!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Data!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Data!$B$2:$B$38</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Data!$C$19:$C$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data (2)'!$A$1:$C$50</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Data (2)'!$A$2:$A$51</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Data (2)'!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Data (2)'!$B$2:$B$38</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Data (2)'!$C$19:$C$22</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Data!$A$2:$A$51</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Data!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Data!$B$2:$B$38</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Data!$C$19:$C$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="2" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Row Labels</t>
   </si>
@@ -75,6 +82,36 @@
   </si>
   <si>
     <t>41-50</t>
+  </si>
+  <si>
+    <t>Count of 37</t>
+  </si>
+  <si>
+    <t>Count of 25</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Sigma</t>
+  </si>
+  <si>
+    <t>Series 1 Stats</t>
+  </si>
+  <si>
+    <t>Series 2 Stats</t>
+  </si>
+  <si>
+    <t>Bins</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -140,6 +177,540 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Randomized Data Points</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Data (2)'!$E$8:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data (2)'!$F$8:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A4A4-4FF8-AB63-622393F7B4E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Data (2)'!$E$8:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data (2)'!$H$8:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A4A4-4FF8-AB63-622393F7B4E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="70"/>
+        <c:axId val="548567056"/>
+        <c:axId val="548567376"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="548567056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Data Value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="548567376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="548567376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frequency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="548567056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1391,20 +1962,20 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1631,8 +2202,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1659,8 +2270,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1761,7 +2372,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1793,10 +2404,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2117,6 +2728,511 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -2147,7 +3263,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2656,6 +3772,47 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>564312</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>129396</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>143774</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>106392</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5024461D-DDD0-4A64-B329-E3CF672D7DA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2740,7 +3897,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3104790" y="5654327"/>
+              <a:off x="3104790" y="5852447"/>
               <a:ext cx="5907656" cy="2974676"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2866,6 +4023,27 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Vermillion" refreshedDate="44051.684032754631" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="49" xr:uid="{5F0B416C-6873-42D1-B9D3-6ED48AEA7261}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B2:C51" sheet="Data"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="37" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="98"/>
+    </cacheField>
+    <cacheField name="25" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="100"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="50">
   <r>
@@ -3115,6 +4293,207 @@
   </r>
   <r>
     <x v="49"/>
+    <n v="61"/>
+    <n v="39"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="49">
+  <r>
+    <n v="7"/>
+    <n v="88"/>
+  </r>
+  <r>
+    <n v="26"/>
+    <n v="65"/>
+  </r>
+  <r>
+    <n v="27"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <n v="91"/>
+    <n v="28"/>
+  </r>
+  <r>
+    <n v="77"/>
+    <n v="51"/>
+  </r>
+  <r>
+    <n v="58"/>
+    <n v="29"/>
+  </r>
+  <r>
+    <n v="87"/>
+    <n v="83"/>
+  </r>
+  <r>
+    <n v="58"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <n v="13"/>
+    <n v="98"/>
+  </r>
+  <r>
+    <n v="62"/>
+    <n v="52"/>
+  </r>
+  <r>
+    <n v="91"/>
+    <n v="26"/>
+  </r>
+  <r>
+    <n v="18"/>
+    <n v="68"/>
+  </r>
+  <r>
+    <n v="18"/>
+    <n v="64"/>
+  </r>
+  <r>
+    <n v="23"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <n v="61"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <n v="90"/>
+    <n v="39"/>
+  </r>
+  <r>
+    <n v="26"/>
+    <n v="53"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <n v="96"/>
+  </r>
+  <r>
+    <n v="54"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <n v="27"/>
+    <n v="40"/>
+  </r>
+  <r>
+    <n v="30"/>
+    <n v="24"/>
+  </r>
+  <r>
+    <n v="52"/>
+    <n v="65"/>
+  </r>
+  <r>
+    <n v="39"/>
+    <n v="27"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <n v="84"/>
+  </r>
+  <r>
+    <n v="37"/>
+    <n v="13"/>
+  </r>
+  <r>
+    <n v="32"/>
+    <n v="83"/>
+  </r>
+  <r>
+    <n v="43"/>
+    <n v="43"/>
+  </r>
+  <r>
+    <n v="28"/>
+    <n v="14"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <n v="65"/>
+  </r>
+  <r>
+    <n v="50"/>
+    <n v="76"/>
+  </r>
+  <r>
+    <n v="50"/>
+    <n v="95"/>
+  </r>
+  <r>
+    <n v="71"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <n v="45"/>
+    <n v="100"/>
+  </r>
+  <r>
+    <n v="37"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <n v="62"/>
+  </r>
+  <r>
+    <n v="84"/>
+    <n v="92"/>
+  </r>
+  <r>
+    <n v="61"/>
+    <n v="58"/>
+  </r>
+  <r>
+    <n v="46"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <n v="51"/>
+    <n v="32"/>
+  </r>
+  <r>
+    <n v="39"/>
+    <n v="9"/>
+  </r>
+  <r>
+    <n v="95"/>
+    <n v="83"/>
+  </r>
+  <r>
+    <n v="16"/>
+    <n v="41"/>
+  </r>
+  <r>
+    <n v="27"/>
+    <n v="99"/>
+  </r>
+  <r>
+    <n v="28"/>
+    <n v="46"/>
+  </r>
+  <r>
+    <n v="89"/>
+    <n v="32"/>
+  </r>
+  <r>
+    <n v="54"/>
+    <n v="19"/>
+  </r>
+  <r>
+    <n v="98"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="98"/>
+    <n v="13"/>
+  </r>
+  <r>
     <n v="61"/>
     <n v="39"/>
   </r>
@@ -3122,7 +4501,44 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{38C5BB80-E974-42CE-9DD0-85C2AC69A4FC}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B77A4207-578B-4C8E-AB02-B1DD900D17F6}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="K16:L17" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Count of 37" fld="0" subtotal="count" baseField="0" baseItem="1"/>
+    <dataField name="Count of 25" fld="1" subtotal="count" baseField="0" baseItem="1"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{38C5BB80-E974-42CE-9DD0-85C2AC69A4FC}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="K6:M12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -3392,20 +4808,890 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B6260C-0ECB-4C8A-A850-02200D43091C}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:H51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="46" width="3" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1">
+        <f>MIN(B2:B51)</f>
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1">
+        <f>MIN(C2:C51)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>88</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1">
+        <f>AVERAGE(B2:B51)</f>
+        <v>46.84</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3">
+        <f>AVERAGE(C2:C51)</f>
+        <v>45.78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>26</v>
+      </c>
+      <c r="C4" s="1">
+        <v>65</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1">
+        <f>MAX(B2:B51)</f>
+        <v>98</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <f>MAX(C2:C51)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1">
+        <f>_xlfn.STDEV.S(B2:B51)</f>
+        <v>27.410231964113887</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5">
+        <f>_xlfn.STDEV.S(C2:C51)</f>
+        <v>31.15746053417665</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>91</v>
+      </c>
+      <c r="C6" s="1">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>77</v>
+      </c>
+      <c r="C7" s="1">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>58</v>
+      </c>
+      <c r="C8" s="1">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <f>COUNTIF($B$2:$B$51,"&gt;="&amp;E8)-COUNTIF($B$2:$B$51,"&gt;="&amp;E9)</f>
+        <v>9</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <f>COUNTIF($C$2:$C$51,"&gt;="&amp;G8)-COUNTIF($C$2:$C$51,"&gt;="&amp;G9)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>87</v>
+      </c>
+      <c r="C9" s="1">
+        <v>83</v>
+      </c>
+      <c r="E9" s="1">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" ref="F9:H13" si="0">COUNTIF($B$2:$B$51,"&gt;="&amp;E9)-COUNTIF($B$2:$B$51,"&gt;="&amp;E10)</f>
+        <v>15</v>
+      </c>
+      <c r="G9" s="1">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" ref="H9:H13" si="1">COUNTIF($C$2:$C$51,"&gt;="&amp;G9)-COUNTIF($C$2:$C$51,"&gt;="&amp;G10)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>58</v>
+      </c>
+      <c r="C10" s="1">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1">
+        <v>40</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G10" s="1">
+        <v>40</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1">
+        <v>98</v>
+      </c>
+      <c r="E11" s="1">
+        <v>60</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G11" s="1">
+        <v>60</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>62</v>
+      </c>
+      <c r="C12" s="1">
+        <v>52</v>
+      </c>
+      <c r="E12" s="1">
+        <v>80</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="G12" s="1">
+        <v>80</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>91</v>
+      </c>
+      <c r="C13" s="1">
+        <v>26</v>
+      </c>
+      <c r="E13" s="1">
+        <v>100</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>100</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1">
+        <v>68</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1">
+        <v>64</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>23</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>61</v>
+      </c>
+      <c r="C17" s="1">
+        <v>6</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>90</v>
+      </c>
+      <c r="C18" s="1">
+        <v>39</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>26</v>
+      </c>
+      <c r="C19" s="1">
+        <v>53</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>96</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>54</v>
+      </c>
+      <c r="C21" s="1">
+        <v>15</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>27</v>
+      </c>
+      <c r="C22" s="1">
+        <v>40</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>30</v>
+      </c>
+      <c r="C23" s="1">
+        <v>24</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>52</v>
+      </c>
+      <c r="C24" s="1">
+        <v>65</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>39</v>
+      </c>
+      <c r="C25" s="1">
+        <v>27</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>84</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>37</v>
+      </c>
+      <c r="C27" s="1">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>32</v>
+      </c>
+      <c r="C28" s="1">
+        <v>83</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1">
+        <v>43</v>
+      </c>
+      <c r="C29" s="1">
+        <v>43</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1">
+        <v>28</v>
+      </c>
+      <c r="C30" s="1">
+        <v>14</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1">
+        <v>6</v>
+      </c>
+      <c r="C31" s="1">
+        <v>65</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1">
+        <v>50</v>
+      </c>
+      <c r="C32" s="1">
+        <v>76</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1">
+        <v>50</v>
+      </c>
+      <c r="C33" s="1">
+        <v>95</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1">
+        <v>71</v>
+      </c>
+      <c r="C34" s="1">
+        <v>15</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1">
+        <v>45</v>
+      </c>
+      <c r="C35" s="1">
+        <v>100</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1">
+        <v>37</v>
+      </c>
+      <c r="C36" s="1">
+        <v>5</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1">
+        <v>19</v>
+      </c>
+      <c r="C37" s="1">
+        <v>62</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1">
+        <v>84</v>
+      </c>
+      <c r="C38" s="1">
+        <v>92</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1">
+        <v>61</v>
+      </c>
+      <c r="C39" s="1">
+        <v>58</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1">
+        <v>46</v>
+      </c>
+      <c r="C40" s="1">
+        <v>10</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1">
+        <v>51</v>
+      </c>
+      <c r="C41" s="1">
+        <v>32</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1">
+        <v>39</v>
+      </c>
+      <c r="C42" s="1">
+        <v>9</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1">
+        <v>95</v>
+      </c>
+      <c r="C43" s="1">
+        <v>83</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1">
+        <v>16</v>
+      </c>
+      <c r="C44" s="1">
+        <v>41</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1">
+        <v>27</v>
+      </c>
+      <c r="C45" s="1">
+        <v>99</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1">
+        <v>28</v>
+      </c>
+      <c r="C46" s="1">
+        <v>46</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1">
+        <v>89</v>
+      </c>
+      <c r="C47" s="1">
+        <v>32</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1">
+        <v>54</v>
+      </c>
+      <c r="C48" s="1">
+        <v>19</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1">
+        <v>98</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1">
+        <v>98</v>
+      </c>
+      <c r="C50" s="1">
+        <v>13</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1">
+        <v>61</v>
+      </c>
+      <c r="C51" s="1">
+        <v>39</v>
+      </c>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C50" xr:uid="{7983B6A6-DDF1-4BC1-BCB4-8B67460324BD}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C51">
+      <sortCondition ref="A1:A50"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:F51">
+    <sortCondition ref="F2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7:M7"/>
+    <sheetView topLeftCell="A32" zoomScale="106" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="2" bestFit="1" customWidth="1"/>
     <col min="16" max="46" width="3" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="11.5546875" bestFit="1" customWidth="1"/>
@@ -3649,8 +5935,14 @@
       <c r="C16" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3660,8 +5952,14 @@
       <c r="C17" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="K17" s="5">
+        <v>49</v>
+      </c>
+      <c r="L17" s="5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3672,7 +5970,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3683,7 +5981,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3694,7 +5992,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3705,7 +6003,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3716,7 +6014,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3727,7 +6025,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3738,7 +6036,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3749,7 +6047,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3760,7 +6058,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3771,7 +6069,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3782,7 +6080,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3793,7 +6091,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -3804,7 +6102,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -3815,7 +6113,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -4037,6 +6335,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>